<commit_message>
Llegue hasta Cecilia Coronel
</commit_message>
<xml_diff>
--- a/Desafios/04/Pair Programming.xlsx
+++ b/Desafios/04/Pair Programming.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\desarrollo\Bootcamp 71241\Desafios\04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB704F1-5D08-4650-953D-DB5AF90CFD8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769F6B36-E509-4AAC-959E-C9C6E5BA2958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -177,7 +177,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -208,12 +208,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="6">
     <border>
@@ -300,15 +294,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -342,7 +327,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -627,8 +621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="36.6" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -642,238 +636,238 @@
   <sheetData>
     <row r="1" spans="2:5" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:5" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="5"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="16"/>
     </row>
     <row r="3" spans="2:5" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B4" s="8">
+      <c r="B4" s="5">
         <v>1</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B5" s="8">
+      <c r="B5" s="5">
         <v>2</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B6" s="8">
+      <c r="B6" s="5">
         <v>3</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B7" s="8">
+      <c r="B7" s="12">
         <v>4</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="17" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B8" s="8">
+      <c r="B8" s="12">
         <v>5</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="13" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B9" s="15">
+      <c r="B9" s="12">
         <v>6</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="13" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B10" s="8">
+      <c r="B10" s="5">
         <v>7</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B11" s="8">
+      <c r="B11" s="12">
         <v>8</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="13" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B12" s="8">
+      <c r="B12" s="5">
         <v>9</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B13" s="8">
+      <c r="B13" s="12">
         <v>10</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="13" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B14" s="8">
+      <c r="B14" s="12">
         <v>11</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="9" t="s">
-        <v>17</v>
-      </c>
+      <c r="D14" s="13"/>
       <c r="E14" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B15" s="8">
+      <c r="B15" s="12">
         <v>12</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="13" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B16" s="8">
+      <c r="B16" s="5">
         <v>13</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B17" s="8">
+      <c r="B17" s="5">
         <v>14</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B18" s="8">
+      <c r="B18" s="5">
         <v>15</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B19" s="8">
+      <c r="B19" s="5">
         <v>16</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B20" s="8">
+      <c r="B20" s="5">
         <v>17</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B21" s="8">
+      <c r="B21" s="5">
         <v>18</v>
       </c>
-      <c r="C21" s="12"/>
-      <c r="D21" s="13"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="10"/>
     </row>
     <row r="22" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B22" s="8">
+      <c r="B22" s="5">
         <v>19</v>
       </c>
-      <c r="C22" s="12"/>
-      <c r="D22" s="13"/>
+      <c r="C22" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="10"/>
     </row>
     <row r="23" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B23" s="8">
+      <c r="B23" s="5">
         <v>20</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
     </row>
     <row r="24" spans="2:4" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B24" s="14"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>